<commit_message>
test of safari window inside the app
</commit_message>
<xml_diff>
--- a/myPlan.xlsx
+++ b/myPlan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="53">
   <si>
     <t>اسم الطالب</t>
   </si>
@@ -58,139 +58,115 @@
     <t>تاريخ الانجاز</t>
   </si>
   <si>
-    <t>النِّسَاء 1</t>
+    <t>الوَاقِعة 1</t>
   </si>
   <si>
     <t>---</t>
   </si>
   <si>
-    <t>الأعرَاف 1</t>
-  </si>
-  <si>
-    <t>الأعرَاف 11</t>
-  </si>
-  <si>
-    <t>الأعرَاف 20</t>
-  </si>
-  <si>
-    <t>الأعرَاف 27</t>
-  </si>
-  <si>
-    <t>الأعرَاف 33</t>
-  </si>
-  <si>
-    <t>الأعرَاف 38</t>
-  </si>
-  <si>
-    <t>الأعرَاف 43</t>
-  </si>
-  <si>
-    <t>الأعرَاف 50</t>
-  </si>
-  <si>
-    <t>الأعرَاف 54</t>
-  </si>
-  <si>
-    <t>الأعرَاف 61</t>
-  </si>
-  <si>
-    <t>الأعرَاف 69</t>
+    <t>الطَّلَاق 1</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 2</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 3</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 4</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 5</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 6</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 7</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 8</t>
   </si>
   <si>
     <t>* أحسنت لقد اجتزت ربع الخطة *</t>
   </si>
   <si>
-    <t>الأعرَاف 73</t>
-  </si>
-  <si>
-    <t>الأعرَاف 79</t>
-  </si>
-  <si>
-    <t>الأعرَاف 85</t>
-  </si>
-  <si>
-    <t>الأعرَاف 89</t>
-  </si>
-  <si>
-    <t>الأعرَاف 96</t>
-  </si>
-  <si>
-    <t>الأعرَاف 104</t>
-  </si>
-  <si>
-    <t>الأعرَاف 116</t>
-  </si>
-  <si>
-    <t>الأعرَاف 127</t>
-  </si>
-  <si>
-    <t>الأعرَاف 133</t>
-  </si>
-  <si>
-    <t>الأعرَاف 138</t>
+    <t>الطَّلَاق 10</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 11</t>
+  </si>
+  <si>
+    <t>الطَّلَاق 12</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 2</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 3</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 4</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 5</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 6</t>
   </si>
   <si>
     <t>* ممتاز لقد اجتزت نصف الخطة *</t>
   </si>
   <si>
-    <t>الأعرَاف 143</t>
-  </si>
-  <si>
-    <t>الأعرَاف 148</t>
-  </si>
-  <si>
-    <t>الأعرَاف 153</t>
-  </si>
-  <si>
-    <t>الأعرَاف 157</t>
-  </si>
-  <si>
-    <t>الأعرَاف 160</t>
-  </si>
-  <si>
-    <t>الأعرَاف 163</t>
-  </si>
-  <si>
-    <t>الأعرَاف 169</t>
-  </si>
-  <si>
-    <t>الأعرَاف 175</t>
-  </si>
-  <si>
-    <t>الأعرَاف 181</t>
-  </si>
-  <si>
-    <t>الأعرَاف 188</t>
+    <t>التَّحرِيم 7</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 8</t>
+  </si>
+  <si>
+    <t>الخ</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 9</t>
+  </si>
+  <si>
+    <t>الرَّحمٰن 1</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 10</t>
+  </si>
+  <si>
+    <t>التَّحرِيم 11</t>
   </si>
   <si>
     <t>* ما شاء الله أنت على وشك الإنتهاء من الخطة *</t>
   </si>
   <si>
-    <t>الأعرَاف 195</t>
-  </si>
-  <si>
-    <t>الأعرَاف 204</t>
-  </si>
-  <si>
-    <t>الأنفَال 4</t>
-  </si>
-  <si>
-    <t>الأنفَال 11</t>
-  </si>
-  <si>
-    <t>الأنفَال 17</t>
-  </si>
-  <si>
-    <t>الأنفَال 25</t>
-  </si>
-  <si>
-    <t>الخ</t>
-  </si>
-  <si>
-    <t>الأنفَال 31</t>
-  </si>
-  <si>
-    <t>آل عِمران 1</t>
+    <t>التَّحرِيم 12</t>
+  </si>
+  <si>
+    <t>المُلك 2</t>
+  </si>
+  <si>
+    <t>المُلك 3</t>
+  </si>
+  <si>
+    <t>المُلك 4</t>
+  </si>
+  <si>
+    <t>المُلك 5</t>
+  </si>
+  <si>
+    <t>المُلك 8</t>
+  </si>
+  <si>
+    <t>المُلك 9</t>
+  </si>
+  <si>
+    <t>المُلك 12</t>
+  </si>
+  <si>
+    <t>المُلك 14</t>
   </si>
   <si>
     <t>* مبارك عليك هذا الإنجاز ومزيد من التقدم والتفوق بإذن الله *</t>
@@ -717,7 +693,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -732,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -741,10 +717,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -759,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
@@ -768,10 +744,10 @@
         <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -786,7 +762,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
@@ -795,10 +771,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -813,19 +789,19 @@
         <v>15</v>
       </c>
       <c r="D7" s="3">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -840,7 +816,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
@@ -849,10 +825,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -867,7 +843,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="3">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
@@ -876,10 +852,10 @@
         <v>16</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -894,7 +870,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="3">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>16</v>
@@ -903,10 +879,10 @@
         <v>16</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -921,7 +897,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>16</v>
@@ -930,10 +906,10 @@
         <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -948,7 +924,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="3">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>16</v>
@@ -957,10 +933,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -970,7 +946,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -990,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="3">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>16</v>
@@ -999,10 +975,10 @@
         <v>16</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1017,7 +993,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="3">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>16</v>
@@ -1026,10 +1002,10 @@
         <v>16</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1044,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>16</v>
@@ -1053,10 +1029,10 @@
         <v>16</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1071,7 +1047,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>16</v>
@@ -1080,10 +1056,10 @@
         <v>16</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1098,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="3">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>16</v>
@@ -1107,10 +1083,10 @@
         <v>16</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1125,7 +1101,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="3">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>16</v>
@@ -1134,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1152,7 +1128,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="3">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>16</v>
@@ -1161,10 +1137,10 @@
         <v>16</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -1179,7 +1155,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="3">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>16</v>
@@ -1188,10 +1164,10 @@
         <v>16</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1206,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="3">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>16</v>
@@ -1215,10 +1191,10 @@
         <v>16</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1233,7 +1209,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="3">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>16</v>
@@ -1242,10 +1218,10 @@
         <v>16</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1255,7 +1231,7 @@
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1275,7 +1251,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="3">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>16</v>
@@ -1284,10 +1260,10 @@
         <v>16</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1302,7 +1278,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="3">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>16</v>
@@ -1311,10 +1287,10 @@
         <v>16</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1329,7 +1305,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="3">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>16</v>
@@ -1338,10 +1314,10 @@
         <v>16</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1355,8 +1331,8 @@
       <c r="C28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="3">
-        <v>108</v>
+      <c r="D28" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>16</v>
@@ -1365,10 +1341,10 @@
         <v>16</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1380,22 +1356,22 @@
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D29" s="3">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1407,22 +1383,22 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -1434,22 +1410,22 @@
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D31" s="3">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -1461,10 +1437,10 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D32" s="3">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>16</v>
@@ -1473,10 +1449,10 @@
         <v>16</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -1488,10 +1464,10 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D33" s="3">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>16</v>
@@ -1500,10 +1476,10 @@
         <v>16</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -1515,10 +1491,10 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D34" s="3">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>16</v>
@@ -1527,10 +1503,10 @@
         <v>16</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1540,7 +1516,7 @@
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -1557,10 +1533,10 @@
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D36" s="3">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>16</v>
@@ -1569,10 +1545,10 @@
         <v>16</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -1584,10 +1560,10 @@
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D37" s="3">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>16</v>
@@ -1596,10 +1572,10 @@
         <v>16</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -1611,10 +1587,10 @@
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D38" s="3">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>16</v>
@@ -1623,10 +1599,10 @@
         <v>16</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -1638,10 +1614,10 @@
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D39" s="3">
-        <v>163</v>
+        <v>35</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>16</v>
@@ -1650,10 +1626,10 @@
         <v>16</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -1665,10 +1641,10 @@
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D40" s="3">
-        <v>170</v>
+        <v>38</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>16</v>
@@ -1677,10 +1653,10 @@
         <v>16</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -1692,10 +1668,10 @@
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D41" s="3">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>16</v>
@@ -1704,10 +1680,10 @@
         <v>16</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -1719,10 +1695,10 @@
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+      <c r="D42" s="3">
+        <v>44</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>16</v>
@@ -1731,10 +1707,10 @@
         <v>16</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -1746,22 +1722,22 @@
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D43" s="3">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -1773,22 +1749,22 @@
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D44" s="3">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -1800,22 +1776,22 @@
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D45" s="3">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -1825,7 +1801,7 @@
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="12" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>

</xml_diff>